<commit_message>
Feature 9 und 10
</commit_message>
<xml_diff>
--- a/Testdaten.xlsx
+++ b/Testdaten.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Daten</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Feature6</t>
+  </si>
+  <si>
+    <t>Feature9</t>
+  </si>
+  <si>
+    <t>Feature10</t>
   </si>
 </sst>
 </file>
@@ -343,7 +349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -351,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A2:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,6 +390,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Main 11 und 12
</commit_message>
<xml_diff>
--- a/Testdaten.xlsx
+++ b/Testdaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marku\Documents\Projects\Git\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79671918-FD5B-44CB-9D29-0342B9B4C4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88482A7E-AC72-4AED-906A-7879C36444C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Daten</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Main8</t>
+  </si>
+  <si>
+    <t>Main11</t>
+  </si>
+  <si>
+    <t>Main12</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.76953125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -390,6 +396,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>